<commit_message>
Update dpassive skills import
</commit_message>
<xml_diff>
--- a/resources/data-imports/Kingdom Passive Skills/passive_skills.xlsx
+++ b/resources/data-imports/Kingdom Passive Skills/passive_skills.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="50">
   <si>
     <t>id</t>
   </si>
@@ -147,6 +147,24 @@
   </si>
   <si>
     <t>As you level this skill, your max Steel will increase by 31,000 per level</t>
+  </si>
+  <si>
+    <t>Capital city</t>
+  </si>
+  <si>
+    <t>Allows a player to designate one of their kingdoms per plane, as a Capital City. Capital Cities allows you to manage multiple kingdoms from one central kingdom.</t>
+  </si>
+  <si>
+    <t>Markets and Economy</t>
+  </si>
+  <si>
+    <t>Allows players to create Market Place in thier kingdoms to allow for resources to be ransfered.</t>
+  </si>
+  <si>
+    <t>Moving resources</t>
+  </si>
+  <si>
+    <t>Allows you to request a total of +90,000 resources at max level for a kingdom. By default a kingdom with a market can request, from another kingdom that also has a market, resources in the total of 5,000 or 10,000 is the kingdom being requested has airships. In total this allows you to mvoe 100,000 resources of a single or of all types.</t>
   </si>
 </sst>
 </file>
@@ -486,7 +504,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:L17"/>
+  <dimension ref="A1:L20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -1073,6 +1091,105 @@
         <v>1</v>
       </c>
     </row>
+    <row r="18" spans="1:12">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>44</v>
+      </c>
+      <c r="C18" t="s">
+        <v>45</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18">
+        <v>2</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
+      <c r="I18">
+        <v>3</v>
+      </c>
+      <c r="J18">
+        <v>3</v>
+      </c>
+      <c r="K18">
+        <v>1</v>
+      </c>
+      <c r="L18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>46</v>
+      </c>
+      <c r="C19" t="s">
+        <v>47</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19">
+        <v>2</v>
+      </c>
+      <c r="H19">
+        <v>0</v>
+      </c>
+      <c r="I19">
+        <v>3</v>
+      </c>
+      <c r="J19">
+        <v>3</v>
+      </c>
+      <c r="K19">
+        <v>1</v>
+      </c>
+      <c r="L19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>48</v>
+      </c>
+      <c r="C20" t="s">
+        <v>49</v>
+      </c>
+      <c r="D20">
+        <v>9</v>
+      </c>
+      <c r="E20">
+        <v>2</v>
+      </c>
+      <c r="G20">
+        <v>10000</v>
+      </c>
+      <c r="H20">
+        <v>0</v>
+      </c>
+      <c r="I20">
+        <v>18</v>
+      </c>
+      <c r="J20">
+        <v>1</v>
+      </c>
+      <c r="K20">
+        <v>1</v>
+      </c>
+      <c r="L20">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Quests, passive skills and new building.
</commit_message>
<xml_diff>
--- a/resources/data-imports/Kingdom Passive Skills/passive_skills.xlsx
+++ b/resources/data-imports/Kingdom Passive Skills/passive_skills.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="46">
   <si>
     <t>id</t>
   </si>
@@ -149,22 +149,10 @@
     <t>As you level this skill, your max Steel will increase by 31,000 per level</t>
   </si>
   <si>
-    <t>Capital city</t>
-  </si>
-  <si>
-    <t>Allows a player to designate one of their kingdoms per plane, as a Capital City. Capital Cities allows you to manage multiple kingdoms from one central kingdom.</t>
-  </si>
-  <si>
-    <t>Markets and Economy</t>
-  </si>
-  <si>
-    <t>Allows players to create Market Place in thier kingdoms to allow for resources to be ransfered.</t>
-  </si>
-  <si>
-    <t>Moving resources</t>
-  </si>
-  <si>
-    <t>Allows you to request a total of +90,000 resources at max level for a kingdom. By default a kingdom with a market can request, from another kingdom that also has a market, resources in the total of 5,000 or 10,000 is the kingdom being requested has airships. In total this allows you to mvoe 100,000 resources of a single or of all types.</t>
+    <t>Market Place</t>
+  </si>
+  <si>
+    <t>Allows players to build and upgrade the Market Place building for their kingdoms. Each kingdom that has a Market Place leveled to level 5, can then request resources from other kingdoms you own, on the same plane - who also have a Market Place at level 5.</t>
   </si>
 </sst>
 </file>
@@ -504,7 +492,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:L20"/>
+  <dimension ref="A1:L18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -1108,10 +1096,10 @@
         <v>2</v>
       </c>
       <c r="H18">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I18">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="J18">
         <v>3</v>
@@ -1120,73 +1108,6 @@
         <v>1</v>
       </c>
       <c r="L18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12">
-      <c r="A19">
-        <v>18</v>
-      </c>
-      <c r="B19" t="s">
-        <v>46</v>
-      </c>
-      <c r="C19" t="s">
-        <v>47</v>
-      </c>
-      <c r="D19">
-        <v>1</v>
-      </c>
-      <c r="E19">
-        <v>2</v>
-      </c>
-      <c r="H19">
-        <v>0</v>
-      </c>
-      <c r="I19">
-        <v>3</v>
-      </c>
-      <c r="J19">
-        <v>3</v>
-      </c>
-      <c r="K19">
-        <v>1</v>
-      </c>
-      <c r="L19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12">
-      <c r="A20">
-        <v>19</v>
-      </c>
-      <c r="B20" t="s">
-        <v>48</v>
-      </c>
-      <c r="C20" t="s">
-        <v>49</v>
-      </c>
-      <c r="D20">
-        <v>9</v>
-      </c>
-      <c r="E20">
-        <v>2</v>
-      </c>
-      <c r="G20">
-        <v>10000</v>
-      </c>
-      <c r="H20">
-        <v>0</v>
-      </c>
-      <c r="I20">
-        <v>18</v>
-      </c>
-      <c r="J20">
-        <v>1</v>
-      </c>
-      <c r="K20">
-        <v>1</v>
-      </c>
-      <c r="L20">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Ready to start creating the quests for the two new passive skills
</commit_message>
<xml_diff>
--- a/resources/data-imports/Kingdom Passive Skills/passive_skills.xlsx
+++ b/resources/data-imports/Kingdom Passive Skills/passive_skills.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="52">
   <si>
     <t>id</t>
   </si>
@@ -38,6 +38,12 @@
     <t>resource_bonus_per_level</t>
   </si>
   <si>
+    <t>capital_city_building_request_travel_time_reduction</t>
+  </si>
+  <si>
+    <t>capital_city_unit_request_travel_time_reduction</t>
+  </si>
+  <si>
     <t>effect_type</t>
   </si>
   <si>
@@ -153,6 +159,18 @@
   </si>
   <si>
     <t>Allows players to build and upgrade the Market Place building for their kingdoms. Each kingdom that has a Market Place leveled to level 5, can then request resources from other kingdoms you own, on the same plane - who also have a Market Place at level 5.</t>
+  </si>
+  <si>
+    <t>Capital City Building Requests</t>
+  </si>
+  <si>
+    <t>The requests for repairing or upgrading buildings send out as requests from a capital city will move 15% faster per level for a maximum of a 60% reduction.</t>
+  </si>
+  <si>
+    <t>Capital City Unit Requests</t>
+  </si>
+  <si>
+    <t>When using a capital city to request units be recruited, the time required to travel will be reduced by 15% per level for a max of 60% time reduction.</t>
   </si>
 </sst>
 </file>
@@ -492,7 +510,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:L18"/>
+  <dimension ref="A1:N20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -501,20 +519,22 @@
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="1" max="1" width="3.428" bestFit="true" customWidth="true" style="0"/>
-    <col min="2" max="2" width="29.421" bestFit="true" customWidth="true" style="0"/>
+    <col min="2" max="2" width="36.42" bestFit="true" customWidth="true" style="0"/>
     <col min="3" max="3" width="469.457" bestFit="true" customWidth="true" style="0"/>
     <col min="4" max="4" width="11.711" bestFit="true" customWidth="true" style="0"/>
     <col min="5" max="5" width="18.71" bestFit="true" customWidth="true" style="0"/>
     <col min="6" max="6" width="18.71" bestFit="true" customWidth="true" style="0"/>
     <col min="7" max="7" width="29.421" bestFit="true" customWidth="true" style="0"/>
-    <col min="8" max="8" width="13.997" bestFit="true" customWidth="true" style="0"/>
-    <col min="9" max="9" width="18.71" bestFit="true" customWidth="true" style="0"/>
-    <col min="10" max="10" width="19.995" bestFit="true" customWidth="true" style="0"/>
-    <col min="11" max="11" width="11.711" bestFit="true" customWidth="true" style="0"/>
-    <col min="12" max="12" width="11.711" bestFit="true" customWidth="true" style="0"/>
+    <col min="8" max="8" width="61.271" bestFit="true" customWidth="true" style="0"/>
+    <col min="9" max="9" width="56.558" bestFit="true" customWidth="true" style="0"/>
+    <col min="10" max="10" width="13.997" bestFit="true" customWidth="true" style="0"/>
+    <col min="11" max="11" width="18.71" bestFit="true" customWidth="true" style="0"/>
+    <col min="12" max="12" width="19.995" bestFit="true" customWidth="true" style="0"/>
+    <col min="13" max="13" width="11.711" bestFit="true" customWidth="true" style="0"/>
+    <col min="14" max="14" width="11.711" bestFit="true" customWidth="true" style="0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:14">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -551,16 +571,22 @@
       <c r="L1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:12">
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D2">
         <v>5</v>
@@ -571,22 +597,22 @@
       <c r="F2">
         <v>0.05</v>
       </c>
-      <c r="H2">
+      <c r="J2">
         <v>0</v>
       </c>
-      <c r="L2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12">
+      <c r="N2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C3" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D3">
         <v>5</v>
@@ -597,28 +623,28 @@
       <c r="F3">
         <v>0.08</v>
       </c>
-      <c r="H3">
-        <v>1</v>
-      </c>
-      <c r="I3">
-        <v>1</v>
-      </c>
       <c r="J3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:12">
+      <c r="L3">
+        <v>2</v>
+      </c>
+      <c r="M3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C4" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D4">
         <v>5</v>
@@ -629,28 +655,28 @@
       <c r="F4">
         <v>0.06</v>
       </c>
-      <c r="H4">
-        <v>3</v>
-      </c>
-      <c r="I4">
-        <v>1</v>
-      </c>
       <c r="J4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:12">
+      <c r="L4">
+        <v>4</v>
+      </c>
+      <c r="M4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C5" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D5">
         <v>5</v>
@@ -661,28 +687,28 @@
       <c r="F5">
         <v>0.06</v>
       </c>
-      <c r="H5">
-        <v>2</v>
-      </c>
-      <c r="I5">
-        <v>1</v>
-      </c>
       <c r="J5">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="K5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:12">
+      <c r="L5">
+        <v>5</v>
+      </c>
+      <c r="M5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C6" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -693,28 +719,28 @@
       <c r="F6">
         <v>0</v>
       </c>
-      <c r="H6">
-        <v>4</v>
-      </c>
-      <c r="I6">
-        <v>3</v>
-      </c>
       <c r="J6">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="K6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12">
+        <v>3</v>
+      </c>
+      <c r="L6">
+        <v>2</v>
+      </c>
+      <c r="M6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C7" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D7">
         <v>5</v>
@@ -725,28 +751,28 @@
       <c r="F7">
         <v>0.07</v>
       </c>
-      <c r="H7">
-        <v>5</v>
-      </c>
-      <c r="I7">
-        <v>3</v>
-      </c>
       <c r="J7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="K7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12">
+        <v>3</v>
+      </c>
+      <c r="L7">
+        <v>4</v>
+      </c>
+      <c r="M7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C8" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -757,31 +783,31 @@
       <c r="F8">
         <v>0</v>
       </c>
-      <c r="H8">
-        <v>4</v>
-      </c>
-      <c r="I8">
+      <c r="J8">
+        <v>4</v>
+      </c>
+      <c r="K8">
         <v>6</v>
       </c>
-      <c r="J8">
-        <v>5</v>
-      </c>
-      <c r="K8">
-        <v>1</v>
-      </c>
       <c r="L8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12">
+        <v>5</v>
+      </c>
+      <c r="M8">
+        <v>1</v>
+      </c>
+      <c r="N8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C9" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D9">
         <v>5</v>
@@ -792,28 +818,28 @@
       <c r="F9">
         <v>0.07</v>
       </c>
-      <c r="H9">
+      <c r="J9">
         <v>6</v>
       </c>
-      <c r="I9">
-        <v>3</v>
-      </c>
-      <c r="J9">
-        <v>3</v>
-      </c>
       <c r="K9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12">
+        <v>3</v>
+      </c>
+      <c r="L9">
+        <v>3</v>
+      </c>
+      <c r="M9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C10" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D10">
         <v>1</v>
@@ -824,28 +850,28 @@
       <c r="F10">
         <v>0</v>
       </c>
-      <c r="H10">
-        <v>4</v>
-      </c>
-      <c r="I10">
+      <c r="J10">
+        <v>4</v>
+      </c>
+      <c r="K10">
         <v>8</v>
       </c>
-      <c r="J10">
-        <v>5</v>
-      </c>
-      <c r="K10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12">
+      <c r="L10">
+        <v>5</v>
+      </c>
+      <c r="M10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C11" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D11">
         <v>1</v>
@@ -856,31 +882,31 @@
       <c r="F11">
         <v>0</v>
       </c>
-      <c r="H11">
-        <v>4</v>
-      </c>
-      <c r="I11">
+      <c r="J11">
+        <v>4</v>
+      </c>
+      <c r="K11">
         <v>6</v>
       </c>
-      <c r="J11">
-        <v>3</v>
-      </c>
-      <c r="K11">
-        <v>1</v>
-      </c>
       <c r="L11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12">
+        <v>3</v>
+      </c>
+      <c r="M11">
+        <v>1</v>
+      </c>
+      <c r="N11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C12" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D12">
         <v>5</v>
@@ -891,31 +917,31 @@
       <c r="F12">
         <v>0.05</v>
       </c>
-      <c r="H12">
+      <c r="J12">
         <v>7</v>
       </c>
-      <c r="I12">
+      <c r="K12">
         <v>10</v>
       </c>
-      <c r="J12">
-        <v>1</v>
-      </c>
-      <c r="K12">
-        <v>1</v>
-      </c>
       <c r="L12">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:12">
+      <c r="M12">
+        <v>1</v>
+      </c>
+      <c r="N12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C13" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D13">
         <v>1</v>
@@ -926,31 +952,31 @@
       <c r="F13">
         <v>0</v>
       </c>
-      <c r="H13">
-        <v>4</v>
-      </c>
-      <c r="I13">
+      <c r="J13">
+        <v>4</v>
+      </c>
+      <c r="K13">
         <v>11</v>
       </c>
-      <c r="J13">
-        <v>2</v>
-      </c>
-      <c r="K13">
-        <v>1</v>
-      </c>
       <c r="L13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12">
+        <v>2</v>
+      </c>
+      <c r="M13">
+        <v>1</v>
+      </c>
+      <c r="N13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C14" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D14">
         <v>6</v>
@@ -961,31 +987,31 @@
       <c r="F14">
         <v>0.03</v>
       </c>
-      <c r="H14">
+      <c r="J14">
         <v>8</v>
       </c>
-      <c r="I14">
+      <c r="K14">
         <v>12</v>
       </c>
-      <c r="J14">
-        <v>1</v>
-      </c>
-      <c r="K14">
-        <v>1</v>
-      </c>
       <c r="L14">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:12">
+      <c r="M14">
+        <v>1</v>
+      </c>
+      <c r="N14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C15" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D15">
         <v>5</v>
@@ -996,31 +1022,31 @@
       <c r="F15">
         <v>0.03</v>
       </c>
-      <c r="H15">
+      <c r="J15">
         <v>9</v>
       </c>
-      <c r="I15">
+      <c r="K15">
         <v>12</v>
       </c>
-      <c r="J15">
-        <v>1</v>
-      </c>
-      <c r="K15">
-        <v>1</v>
-      </c>
       <c r="L15">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:12">
+      <c r="M15">
+        <v>1</v>
+      </c>
+      <c r="N15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C16" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D16">
         <v>8</v>
@@ -1031,31 +1057,31 @@
       <c r="G16">
         <v>31000</v>
       </c>
-      <c r="H16">
+      <c r="J16">
         <v>10</v>
       </c>
-      <c r="I16">
-        <v>2</v>
-      </c>
-      <c r="J16">
-        <v>5</v>
-      </c>
       <c r="K16">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12">
+        <v>5</v>
+      </c>
+      <c r="M16">
+        <v>1</v>
+      </c>
+      <c r="N16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C17" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D17">
         <v>8</v>
@@ -1066,28 +1092,28 @@
       <c r="G17">
         <v>31000</v>
       </c>
-      <c r="H17">
+      <c r="J17">
         <v>11</v>
       </c>
-      <c r="I17">
+      <c r="K17">
         <v>11</v>
       </c>
-      <c r="J17">
-        <v>5</v>
-      </c>
-      <c r="K17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12">
+      <c r="L17">
+        <v>5</v>
+      </c>
+      <c r="M17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C18" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D18">
         <v>1</v>
@@ -1095,19 +1121,89 @@
       <c r="E18">
         <v>2</v>
       </c>
-      <c r="H18">
-        <v>4</v>
-      </c>
-      <c r="I18">
+      <c r="J18">
+        <v>4</v>
+      </c>
+      <c r="K18">
         <v>15</v>
       </c>
-      <c r="J18">
-        <v>3</v>
-      </c>
-      <c r="K18">
-        <v>1</v>
-      </c>
       <c r="L18">
+        <v>3</v>
+      </c>
+      <c r="M18">
+        <v>1</v>
+      </c>
+      <c r="N18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>48</v>
+      </c>
+      <c r="C19" t="s">
+        <v>49</v>
+      </c>
+      <c r="D19">
+        <v>4</v>
+      </c>
+      <c r="E19">
+        <v>3</v>
+      </c>
+      <c r="H19">
+        <v>0.15</v>
+      </c>
+      <c r="J19">
+        <v>12</v>
+      </c>
+      <c r="K19">
+        <v>3</v>
+      </c>
+      <c r="L19">
+        <v>2</v>
+      </c>
+      <c r="M19">
+        <v>1</v>
+      </c>
+      <c r="N19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>50</v>
+      </c>
+      <c r="C20" t="s">
+        <v>51</v>
+      </c>
+      <c r="D20">
+        <v>4</v>
+      </c>
+      <c r="E20">
+        <v>3</v>
+      </c>
+      <c r="I20">
+        <v>0.15</v>
+      </c>
+      <c r="J20">
+        <v>13</v>
+      </c>
+      <c r="K20">
+        <v>4</v>
+      </c>
+      <c r="L20">
+        <v>2</v>
+      </c>
+      <c r="M20">
+        <v>1</v>
+      </c>
+      <c r="N20">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated skills and added quests
</commit_message>
<xml_diff>
--- a/resources/data-imports/Kingdom Passive Skills/passive_skills.xlsx
+++ b/resources/data-imports/Kingdom Passive Skills/passive_skills.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="55">
   <si>
     <t>id</t>
   </si>
@@ -44,6 +44,9 @@
     <t>capital_city_unit_request_travel_time_reduction</t>
   </si>
   <si>
+    <t>resource_request_time_reduction</t>
+  </si>
+  <si>
     <t>effect_type</t>
   </si>
   <si>
@@ -171,6 +174,12 @@
   </si>
   <si>
     <t>When using a capital city to request units be recruited, the time required to travel will be reduced by 15% per level for a max of 60% time reduction.</t>
+  </si>
+  <si>
+    <t>Speedy Resources</t>
+  </si>
+  <si>
+    <t>When requesting resources from other kingdoms, the time to travel between kingdoms will reduce by 15% per level for a max of 60%.</t>
   </si>
 </sst>
 </file>
@@ -510,7 +519,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:N20"/>
+  <dimension ref="A1:O21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -527,14 +536,15 @@
     <col min="7" max="7" width="29.421" bestFit="true" customWidth="true" style="0"/>
     <col min="8" max="8" width="61.271" bestFit="true" customWidth="true" style="0"/>
     <col min="9" max="9" width="56.558" bestFit="true" customWidth="true" style="0"/>
-    <col min="10" max="10" width="13.997" bestFit="true" customWidth="true" style="0"/>
-    <col min="11" max="11" width="18.71" bestFit="true" customWidth="true" style="0"/>
-    <col min="12" max="12" width="19.995" bestFit="true" customWidth="true" style="0"/>
-    <col min="13" max="13" width="11.711" bestFit="true" customWidth="true" style="0"/>
+    <col min="10" max="10" width="37.705" bestFit="true" customWidth="true" style="0"/>
+    <col min="11" max="11" width="13.997" bestFit="true" customWidth="true" style="0"/>
+    <col min="12" max="12" width="18.71" bestFit="true" customWidth="true" style="0"/>
+    <col min="13" max="13" width="19.995" bestFit="true" customWidth="true" style="0"/>
     <col min="14" max="14" width="11.711" bestFit="true" customWidth="true" style="0"/>
+    <col min="15" max="15" width="11.711" bestFit="true" customWidth="true" style="0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -577,16 +587,19 @@
       <c r="N1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" spans="1:14">
+      <c r="O1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D2">
         <v>5</v>
@@ -597,22 +610,22 @@
       <c r="F2">
         <v>0.05</v>
       </c>
-      <c r="J2">
+      <c r="K2">
         <v>0</v>
       </c>
-      <c r="N2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14">
+      <c r="O2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D3">
         <v>5</v>
@@ -623,28 +636,28 @@
       <c r="F3">
         <v>0.08</v>
       </c>
-      <c r="J3">
-        <v>1</v>
-      </c>
       <c r="K3">
         <v>1</v>
       </c>
       <c r="L3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14">
+        <v>2</v>
+      </c>
+      <c r="N3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D4">
         <v>5</v>
@@ -655,28 +668,28 @@
       <c r="F4">
         <v>0.06</v>
       </c>
-      <c r="J4">
-        <v>3</v>
-      </c>
       <c r="K4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L4">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="M4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14">
+        <v>4</v>
+      </c>
+      <c r="N4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D5">
         <v>5</v>
@@ -687,28 +700,28 @@
       <c r="F5">
         <v>0.06</v>
       </c>
-      <c r="J5">
-        <v>2</v>
-      </c>
       <c r="K5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L5">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="M5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14">
+        <v>5</v>
+      </c>
+      <c r="N5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -719,28 +732,28 @@
       <c r="F6">
         <v>0</v>
       </c>
-      <c r="J6">
-        <v>4</v>
-      </c>
       <c r="K6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="L6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14">
+        <v>2</v>
+      </c>
+      <c r="N6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C7" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D7">
         <v>5</v>
@@ -751,28 +764,28 @@
       <c r="F7">
         <v>0.07</v>
       </c>
-      <c r="J7">
-        <v>5</v>
-      </c>
       <c r="K7">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="L7">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14">
+        <v>4</v>
+      </c>
+      <c r="N7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -783,31 +796,31 @@
       <c r="F8">
         <v>0</v>
       </c>
-      <c r="J8">
-        <v>4</v>
-      </c>
       <c r="K8">
+        <v>4</v>
+      </c>
+      <c r="L8">
         <v>6</v>
       </c>
-      <c r="L8">
-        <v>5</v>
-      </c>
       <c r="M8">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="N8">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:14">
+      <c r="O8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D9">
         <v>5</v>
@@ -818,28 +831,28 @@
       <c r="F9">
         <v>0.07</v>
       </c>
-      <c r="J9">
+      <c r="K9">
         <v>6</v>
       </c>
-      <c r="K9">
-        <v>3</v>
-      </c>
       <c r="L9">
         <v>3</v>
       </c>
       <c r="M9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14">
+        <v>3</v>
+      </c>
+      <c r="N9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C10" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D10">
         <v>1</v>
@@ -850,28 +863,28 @@
       <c r="F10">
         <v>0</v>
       </c>
-      <c r="J10">
-        <v>4</v>
-      </c>
       <c r="K10">
+        <v>4</v>
+      </c>
+      <c r="L10">
         <v>8</v>
       </c>
-      <c r="L10">
-        <v>5</v>
-      </c>
       <c r="M10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14">
+        <v>5</v>
+      </c>
+      <c r="N10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C11" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D11">
         <v>1</v>
@@ -882,31 +895,31 @@
       <c r="F11">
         <v>0</v>
       </c>
-      <c r="J11">
-        <v>4</v>
-      </c>
       <c r="K11">
+        <v>4</v>
+      </c>
+      <c r="L11">
         <v>6</v>
       </c>
-      <c r="L11">
-        <v>3</v>
-      </c>
       <c r="M11">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="N11">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:14">
+      <c r="O11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C12" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D12">
         <v>5</v>
@@ -917,31 +930,31 @@
       <c r="F12">
         <v>0.05</v>
       </c>
-      <c r="J12">
+      <c r="K12">
         <v>7</v>
       </c>
-      <c r="K12">
+      <c r="L12">
         <v>10</v>
       </c>
-      <c r="L12">
-        <v>1</v>
-      </c>
       <c r="M12">
         <v>1</v>
       </c>
       <c r="N12">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:14">
+      <c r="O12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C13" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D13">
         <v>1</v>
@@ -952,31 +965,31 @@
       <c r="F13">
         <v>0</v>
       </c>
-      <c r="J13">
-        <v>4</v>
-      </c>
       <c r="K13">
+        <v>4</v>
+      </c>
+      <c r="L13">
         <v>11</v>
       </c>
-      <c r="L13">
-        <v>2</v>
-      </c>
       <c r="M13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N13">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:14">
+      <c r="O13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C14" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D14">
         <v>6</v>
@@ -987,31 +1000,31 @@
       <c r="F14">
         <v>0.03</v>
       </c>
-      <c r="J14">
+      <c r="K14">
         <v>8</v>
       </c>
-      <c r="K14">
+      <c r="L14">
         <v>12</v>
       </c>
-      <c r="L14">
-        <v>1</v>
-      </c>
       <c r="M14">
         <v>1</v>
       </c>
       <c r="N14">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:14">
+      <c r="O14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C15" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D15">
         <v>5</v>
@@ -1022,31 +1035,31 @@
       <c r="F15">
         <v>0.03</v>
       </c>
-      <c r="J15">
+      <c r="K15">
         <v>9</v>
       </c>
-      <c r="K15">
+      <c r="L15">
         <v>12</v>
       </c>
-      <c r="L15">
-        <v>1</v>
-      </c>
       <c r="M15">
         <v>1</v>
       </c>
       <c r="N15">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:14">
+      <c r="O15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C16" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D16">
         <v>8</v>
@@ -1057,31 +1070,31 @@
       <c r="G16">
         <v>31000</v>
       </c>
-      <c r="J16">
+      <c r="K16">
         <v>10</v>
       </c>
-      <c r="K16">
-        <v>2</v>
-      </c>
       <c r="L16">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="M16">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="N16">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:14">
+      <c r="O16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C17" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D17">
         <v>8</v>
@@ -1092,28 +1105,28 @@
       <c r="G17">
         <v>31000</v>
       </c>
-      <c r="J17">
-        <v>11</v>
-      </c>
       <c r="K17">
         <v>11</v>
       </c>
       <c r="L17">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="M17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14">
+        <v>5</v>
+      </c>
+      <c r="N17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C18" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D18">
         <v>1</v>
@@ -1121,31 +1134,31 @@
       <c r="E18">
         <v>2</v>
       </c>
-      <c r="J18">
-        <v>4</v>
-      </c>
       <c r="K18">
+        <v>4</v>
+      </c>
+      <c r="L18">
         <v>15</v>
       </c>
-      <c r="L18">
-        <v>3</v>
-      </c>
       <c r="M18">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="N18">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:14">
+      <c r="O18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C19" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D19">
         <v>4</v>
@@ -1156,31 +1169,31 @@
       <c r="H19">
         <v>0.15</v>
       </c>
-      <c r="J19">
+      <c r="K19">
         <v>12</v>
       </c>
-      <c r="K19">
-        <v>3</v>
-      </c>
       <c r="L19">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M19">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N19">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:14">
+      <c r="O19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C20" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D20">
         <v>4</v>
@@ -1191,19 +1204,54 @@
       <c r="I20">
         <v>0.15</v>
       </c>
-      <c r="J20">
+      <c r="K20">
         <v>13</v>
       </c>
-      <c r="K20">
-        <v>4</v>
-      </c>
       <c r="L20">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="M20">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N20">
+        <v>1</v>
+      </c>
+      <c r="O20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>53</v>
+      </c>
+      <c r="C21" t="s">
+        <v>54</v>
+      </c>
+      <c r="D21">
+        <v>4</v>
+      </c>
+      <c r="E21">
+        <v>4</v>
+      </c>
+      <c r="J21">
+        <v>0.15</v>
+      </c>
+      <c r="K21">
+        <v>14</v>
+      </c>
+      <c r="L21">
+        <v>17</v>
+      </c>
+      <c r="M21">
+        <v>1</v>
+      </c>
+      <c r="N21">
+        <v>1</v>
+      </c>
+      <c r="O21">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
More quests and more kingdom passives
</commit_message>
<xml_diff>
--- a/resources/data-imports/Kingdom Passive Skills/passive_skills.xlsx
+++ b/resources/data-imports/Kingdom Passive Skills/passive_skills.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="67">
   <si>
     <t>id</t>
   </si>
@@ -180,6 +180,42 @@
   </si>
   <si>
     <t>When requesting resources from other kingdoms, the time to travel between kingdoms will reduce by 15% per level for a max of 60%.</t>
+  </si>
+  <si>
+    <t>Master Farmer</t>
+  </si>
+  <si>
+    <t>As you level this skill you will get 10% extra population on the hourly update. At level 10, you will gain 100% more population.</t>
+  </si>
+  <si>
+    <t>Master Stone Mason</t>
+  </si>
+  <si>
+    <t>Gain an additonal 10% stone per level for an additional 100% when the hourly update hits.</t>
+  </si>
+  <si>
+    <t>Master Wood Worker</t>
+  </si>
+  <si>
+    <t>Gain an extra 10% wood for a max of 100% on the hourly update.</t>
+  </si>
+  <si>
+    <t>Master of Iron</t>
+  </si>
+  <si>
+    <t>As you level this skill you will gain an additional 10% per level of extra iron for a max of 100% at max level when the hourly update hits.</t>
+  </si>
+  <si>
+    <t>Master of Steel</t>
+  </si>
+  <si>
+    <t>You will gain an additional 10% steel per level for a max of 100% when you smelt steel.</t>
+  </si>
+  <si>
+    <t>Master Potter</t>
+  </si>
+  <si>
+    <t>As you level this skill you will gain 10% more clay per hour on the hourly update for a max of 100% at max level.</t>
   </si>
 </sst>
 </file>
@@ -519,7 +555,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:O21"/>
+  <dimension ref="A1:O27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -1255,6 +1291,216 @@
         <v>1</v>
       </c>
     </row>
+    <row r="22" spans="1:15">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>55</v>
+      </c>
+      <c r="C22" t="s">
+        <v>56</v>
+      </c>
+      <c r="D22">
+        <v>10</v>
+      </c>
+      <c r="E22">
+        <v>1</v>
+      </c>
+      <c r="F22">
+        <v>0.1</v>
+      </c>
+      <c r="K22">
+        <v>15</v>
+      </c>
+      <c r="L22">
+        <v>8</v>
+      </c>
+      <c r="M22">
+        <v>5</v>
+      </c>
+      <c r="N22">
+        <v>1</v>
+      </c>
+      <c r="O22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>57</v>
+      </c>
+      <c r="C23" t="s">
+        <v>58</v>
+      </c>
+      <c r="D23">
+        <v>10</v>
+      </c>
+      <c r="E23">
+        <v>1</v>
+      </c>
+      <c r="F23">
+        <v>0.1</v>
+      </c>
+      <c r="K23">
+        <v>16</v>
+      </c>
+      <c r="L23">
+        <v>15</v>
+      </c>
+      <c r="M23">
+        <v>4</v>
+      </c>
+      <c r="N23">
+        <v>1</v>
+      </c>
+      <c r="O23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>59</v>
+      </c>
+      <c r="C24" t="s">
+        <v>60</v>
+      </c>
+      <c r="D24">
+        <v>10</v>
+      </c>
+      <c r="E24">
+        <v>1</v>
+      </c>
+      <c r="F24">
+        <v>0.1</v>
+      </c>
+      <c r="K24">
+        <v>17</v>
+      </c>
+      <c r="L24">
+        <v>2</v>
+      </c>
+      <c r="M24">
+        <v>3</v>
+      </c>
+      <c r="N24">
+        <v>1</v>
+      </c>
+      <c r="O24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>61</v>
+      </c>
+      <c r="C25" t="s">
+        <v>62</v>
+      </c>
+      <c r="D25">
+        <v>10</v>
+      </c>
+      <c r="E25">
+        <v>2</v>
+      </c>
+      <c r="F25">
+        <v>0.1</v>
+      </c>
+      <c r="K25">
+        <v>18</v>
+      </c>
+      <c r="L25">
+        <v>6</v>
+      </c>
+      <c r="M25">
+        <v>5</v>
+      </c>
+      <c r="N25">
+        <v>1</v>
+      </c>
+      <c r="O25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
+        <v>63</v>
+      </c>
+      <c r="C26" t="s">
+        <v>64</v>
+      </c>
+      <c r="D26">
+        <v>10</v>
+      </c>
+      <c r="E26">
+        <v>3</v>
+      </c>
+      <c r="F26">
+        <v>0.1</v>
+      </c>
+      <c r="K26">
+        <v>20</v>
+      </c>
+      <c r="L26">
+        <v>11</v>
+      </c>
+      <c r="M26">
+        <v>5</v>
+      </c>
+      <c r="N26">
+        <v>1</v>
+      </c>
+      <c r="O26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>65</v>
+      </c>
+      <c r="C27" t="s">
+        <v>66</v>
+      </c>
+      <c r="D27">
+        <v>10</v>
+      </c>
+      <c r="E27">
+        <v>1</v>
+      </c>
+      <c r="F27">
+        <v>0.1</v>
+      </c>
+      <c r="K27">
+        <v>19</v>
+      </c>
+      <c r="L27">
+        <v>2</v>
+      </c>
+      <c r="M27">
+        <v>3</v>
+      </c>
+      <c r="N27">
+        <v>1</v>
+      </c>
+      <c r="O27">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>